<commit_message>
added pre-requisite for Account Lockout
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23420" windowHeight="10320"/>
+    <workbookView windowHeight="4575" windowWidth="18555" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateUser" sheetId="2" r:id="rId2"/>
-    <sheet name="GroupDetails" sheetId="3" r:id="rId3"/>
-    <sheet name="CreateEmployee" sheetId="4" r:id="rId4"/>
+    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
+    <sheet name="CreateUser" r:id="rId2" sheetId="2"/>
+    <sheet name="GroupDetails" r:id="rId3" sheetId="3"/>
+    <sheet name="CreateEmployee" r:id="rId4" sheetId="4"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>Admin</t>
   </si>
@@ -46,9 +47,6 @@
     <t>testlock123</t>
   </si>
   <si>
-    <t>Account Lockout Test</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -164,18 +162,16 @@
   </si>
   <si>
     <t>martink@testmail.com</t>
+  </si>
+  <si>
+    <t>Test invalid password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -225,51 +221,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Comma[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Percent" xfId="4" builtinId="5"/>
-    <cellStyle name="Currency[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -278,10 +264,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -439,7 +425,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -448,13 +434,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -464,7 +450,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -473,7 +459,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -482,7 +468,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -492,12 +478,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -528,7 +514,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -547,7 +533,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -563,13 +549,14 @@
         <a:custGeom>
           <a:avLst/>
           <a:gdLst>
-            <a:gd name="_h" fmla="val 21600"/>
-            <a:gd name="_w" fmla="val 21600"/>
+            <a:gd fmla="val 21600" name="_h"/>
+            <a:gd fmla="val 21600" name="_w"/>
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect b="0" l="0" r="0" t="0"/>
           <a:pathLst>
-            <a:path w="21600" h="21600"/>
+            <a:path h="21600" w="21600"/>
           </a:pathLst>
         </a:custGeom>
         <a:gradFill rotWithShape="0">
@@ -583,7 +570,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="15875">
           <a:solidFill>
             <a:srgbClr val="739CC3"/>
           </a:solidFill>
@@ -600,30 +587,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="20.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="22.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="17.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="16.4285714285714" customWidth="1"/>
-    <col min="7" max="7" width="16.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="14.5714285714286" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="13.2857142857143" customWidth="1"/>
-    <col min="11" max="11" width="14.5714285714286" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -634,7 +620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -652,338 +638,338 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42857142857143" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.8571428571429" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.8571428571429" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.8571428571429" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7142857142857" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="23.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:13">
+    <row customFormat="1" r="1" s="1" spans="1:13">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1">
         <v>1267</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="J2" s="1">
         <v>660675</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1">
         <v>1267</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="J3" s="1">
         <v>660675</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1">
         <v>1267</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="J4" s="1">
         <v>660675</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M4" r:id="rId1" display="martink@testmail.com"/>
-    <hyperlink ref="M3" r:id="rId1" display="martink@testmail.com"/>
-    <hyperlink ref="M2" r:id="rId1" display="martink@testmail.com"/>
+    <hyperlink r:id="rId1" ref="M4"/>
+    <hyperlink r:id="rId2" ref="M3"/>
+    <hyperlink r:id="rId3" ref="M2"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added data to test data
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sameer\Title21Automation\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="23420" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17580" windowHeight="3675" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="CreateUser" sheetId="2" r:id="rId2"/>
     <sheet name="GroupDetails" sheetId="3" r:id="rId3"/>
     <sheet name="CreateEmployee" sheetId="4" r:id="rId4"/>
+    <sheet name="DocumentRoutes" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
   <si>
     <t>Admin</t>
   </si>
@@ -46,9 +52,6 @@
     <t>testlock123</t>
   </si>
   <si>
-    <t>Account Lockout Test</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -164,25 +167,101 @@
   </si>
   <si>
     <t>martink@testmail.com</t>
+  </si>
+  <si>
+    <t>Account Lockout Test - invalid password</t>
+  </si>
+  <si>
+    <t>Account Lockout Test - valid password</t>
+  </si>
+  <si>
+    <t>checkin</t>
+  </si>
+  <si>
+    <t>checkout</t>
+  </si>
+  <si>
+    <t>userperson</t>
+  </si>
+  <si>
+    <t>checkin checkout test</t>
+  </si>
+  <si>
+    <t>test routeneo</t>
+  </si>
+  <si>
+    <t>Sp Tester</t>
+  </si>
+  <si>
+    <t>Group Approvers</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Approver</t>
+  </si>
+  <si>
+    <t>Test Summary</t>
+  </si>
+  <si>
+    <t>PinToApprove</t>
+  </si>
+  <si>
+    <t>RouteName</t>
+  </si>
+  <si>
+    <t>GroupApproverSeq</t>
+  </si>
+  <si>
+    <t>AddApproverGroup</t>
+  </si>
+  <si>
+    <t>GroupAprrovers</t>
+  </si>
+  <si>
+    <t>AllottedDays</t>
+  </si>
+  <si>
+    <t>ApproverSeq</t>
+  </si>
+  <si>
+    <t>AddApprover</t>
+  </si>
+  <si>
+    <t>ApproverLocation</t>
+  </si>
+  <si>
+    <t>ApproverRole</t>
+  </si>
+  <si>
+    <t>DocSummary</t>
+  </si>
+  <si>
+    <t>DocTitle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -225,51 +304,49 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Comma[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Percent" xfId="4" builtinId="5"/>
-    <cellStyle name="Currency[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -568,6 +645,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -600,27 +678,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="20.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="22.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="17.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="16.4285714285714" customWidth="1"/>
-    <col min="7" max="7" width="16.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="14.5714285714286" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="13.2857142857143" customWidth="1"/>
-    <col min="11" max="11" width="14.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -645,345 +722,481 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42857142857143" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.8571428571429" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.8571428571429" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.8571428571429" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7142857142857" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:13">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1">
         <v>1267</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="J2" s="1">
         <v>660675</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1">
         <v>1267</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="J3" s="1">
         <v>660675</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1">
         <v>1267</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="J4" s="1">
         <v>660675</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M4" r:id="rId1" display="martink@testmail.com"/>
-    <hyperlink ref="M3" r:id="rId1" display="martink@testmail.com"/>
-    <hyperlink ref="M2" r:id="rId1" display="martink@testmail.com"/>
+    <hyperlink ref="M4" r:id="rId1"/>
+    <hyperlink ref="M3" r:id="rId2"/>
+    <hyperlink ref="M2" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="19.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="8" width="9.140625" style="5"/>
+    <col min="9" max="9" width="18.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="9.140625" style="5"/>
+    <col min="12" max="12" width="15.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="6">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="6">
+        <v>262829</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
uploading test data file
uploading test data file
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -5,25 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\git\Title21Automation\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neosoft\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateUser" sheetId="2" r:id="rId2"/>
-    <sheet name="GroupDetails" sheetId="3" r:id="rId3"/>
-    <sheet name="CreateEmployee" sheetId="4" r:id="rId4"/>
-    <sheet name="DocumentRoutes" sheetId="5" r:id="rId5"/>
+    <sheet name="Codes" sheetId="6" r:id="rId2"/>
+    <sheet name="CreateUser" sheetId="2" r:id="rId3"/>
+    <sheet name="GroupDetails" sheetId="3" r:id="rId4"/>
+    <sheet name="CreateEmployee" sheetId="4" r:id="rId5"/>
+    <sheet name="DocumentRoutes" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="104">
   <si>
     <t>Admin</t>
   </si>
@@ -295,10 +296,46 @@
     <t>Martink845</t>
   </si>
   <si>
-    <t>reports</t>
-  </si>
-  <si>
-    <t>Reports Test</t>
+    <t>Test case code</t>
+  </si>
+  <si>
+    <t>Test case sp code</t>
+  </si>
+  <si>
+    <t>AlreadyUsedClassName</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>CodesName</t>
+  </si>
+  <si>
+    <t>CodesId</t>
+  </si>
+  <si>
+    <t>TestCaseCodesString</t>
+  </si>
+  <si>
+    <t>Summary test</t>
+  </si>
+  <si>
+    <t>CodesDefinition</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>CritId</t>
+  </si>
+  <si>
+    <t>Test doc class</t>
+  </si>
+  <si>
+    <t>OtherCodeClassFromCodeClass</t>
+  </si>
+  <si>
+    <t>IndxCard</t>
   </si>
 </sst>
 </file>
@@ -752,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -931,17 +968,6 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -950,6 +976,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1049,7 +1146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1082,7 +1179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
@@ -1320,7 +1417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated code for the periodic review
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\git\Title21Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView windowHeight="7755" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="Codes" sheetId="6" r:id="rId2"/>
-    <sheet name="CreateUser" sheetId="2" r:id="rId3"/>
-    <sheet name="GroupDetails" sheetId="3" r:id="rId4"/>
-    <sheet name="CreateEmployee" sheetId="4" r:id="rId5"/>
-    <sheet name="DocumentRoutes" sheetId="5" r:id="rId6"/>
+    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
+    <sheet name="Codes" r:id="rId2" sheetId="6"/>
+    <sheet name="CreateUser" r:id="rId3" sheetId="2"/>
+    <sheet name="GroupDetails" r:id="rId4" sheetId="3"/>
+    <sheet name="CreateEmployee" r:id="rId5" sheetId="4"/>
+    <sheet name="DocumentRoutes" r:id="rId6" sheetId="5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
@@ -354,6 +354,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -418,49 +419,49 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -477,10 +478,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -638,7 +639,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -647,13 +648,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -663,7 +664,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -672,7 +673,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -681,7 +682,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -691,12 +692,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -727,7 +728,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -746,7 +747,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -762,14 +763,14 @@
         <a:custGeom>
           <a:avLst/>
           <a:gdLst>
-            <a:gd name="_h" fmla="val 21600"/>
-            <a:gd name="_w" fmla="val 21600"/>
+            <a:gd fmla="val 21600" name="_h"/>
+            <a:gd fmla="val 21600" name="_w"/>
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:rect b="0" l="0" r="0" t="0"/>
           <a:pathLst>
-            <a:path w="21600" h="21600"/>
+            <a:path h="21600" w="21600"/>
           </a:pathLst>
         </a:custGeom>
         <a:gradFill rotWithShape="0">
@@ -783,7 +784,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="15875">
           <a:solidFill>
             <a:srgbClr val="739CC3"/>
           </a:solidFill>
@@ -800,8 +801,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -809,17 +810,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="39.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="15.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="14.5703125" collapsed="true"/>
+    <col min="12" max="16384" style="4" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1003,15 +1004,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -1019,8 +1020,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1076,13 +1077,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -1090,17 +1091,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1174,15 +1175,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
@@ -1207,15 +1208,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -1223,22 +1224,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="23.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
+    <row customFormat="1" r="1" s="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1441,19 +1442,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M4" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
-    <hyperlink ref="M2" r:id="rId3"/>
+    <hyperlink r:id="rId1" ref="M4"/>
+    <hyperlink r:id="rId2" ref="M3"/>
+    <hyperlink r:id="rId3" ref="M2"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId4"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -1461,22 +1462,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="5" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18" style="5" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="17" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="2" style="5" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="21.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="16.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="5" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="15.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="5" width="18.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="19.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="5" width="17.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="5" width="18.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="8" width="18.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="5" width="14.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="5" width="13.5703125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="5" width="11.7109375" collapsed="true"/>
+    <col min="17" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1562,7 +1563,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new testcase for the NotOwned doc
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neosoft\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="7755" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="AuditLogsDetails" sheetId="7" r:id="rId2"/>
-    <sheet name="Codes" sheetId="6" r:id="rId3"/>
-    <sheet name="CreateUser" sheetId="2" r:id="rId4"/>
-    <sheet name="GroupDetails" sheetId="3" r:id="rId5"/>
-    <sheet name="CreateEmployee" sheetId="4" r:id="rId6"/>
-    <sheet name="DocumentRoutes" sheetId="5" r:id="rId7"/>
+    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
+    <sheet name="AuditLogsDetails" r:id="rId2" sheetId="7"/>
+    <sheet name="Codes" r:id="rId3" sheetId="6"/>
+    <sheet name="CreateUser" r:id="rId4" sheetId="2"/>
+    <sheet name="GroupDetails" r:id="rId5" sheetId="3"/>
+    <sheet name="CreateEmployee" r:id="rId6" sheetId="4"/>
+    <sheet name="DocumentRoutes" r:id="rId7" sheetId="5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
@@ -370,6 +370,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -434,49 +435,49 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -493,10 +494,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -654,7 +655,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -663,13 +664,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -679,7 +680,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -688,7 +689,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -697,7 +698,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -707,12 +708,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -743,7 +744,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -762,7 +763,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -778,14 +779,14 @@
         <a:custGeom>
           <a:avLst/>
           <a:gdLst>
-            <a:gd name="_h" fmla="val 21600"/>
-            <a:gd name="_w" fmla="val 21600"/>
+            <a:gd fmla="val 21600" name="_h"/>
+            <a:gd fmla="val 21600" name="_w"/>
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:rect b="0" l="0" r="0" t="0"/>
           <a:pathLst>
-            <a:path w="21600" h="21600"/>
+            <a:path h="21600" w="21600"/>
           </a:pathLst>
         </a:custGeom>
         <a:gradFill rotWithShape="0">
@@ -799,7 +800,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="15875">
           <a:solidFill>
             <a:srgbClr val="739CC3"/>
           </a:solidFill>
@@ -816,8 +817,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -825,17 +826,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="39.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="15.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="14.5703125" collapsed="true"/>
+    <col min="12" max="16384" style="4" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1019,15 +1020,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
@@ -1059,13 +1060,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -1073,8 +1074,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1130,13 +1131,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -1144,17 +1145,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1228,15 +1229,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
@@ -1261,15 +1262,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -1277,22 +1278,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="23.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
+    <row customFormat="1" r="1" s="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1495,19 +1496,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M4" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
-    <hyperlink ref="M2" r:id="rId3"/>
+    <hyperlink r:id="rId1" ref="M4"/>
+    <hyperlink r:id="rId2" ref="M3"/>
+    <hyperlink r:id="rId3" ref="M2"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId4"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -1515,22 +1516,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="5" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18" style="5" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="17" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="2" style="5" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="21.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="16.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="5" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="15.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="5" width="18.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="19.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="5" width="17.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="5" width="18.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="8" width="18.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="5" width="14.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="5" width="13.5703125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="5" width="11.7109375" collapsed="true"/>
+    <col min="17" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1616,7 +1617,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding files to sync with onsite repo
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="7755" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="6" firstSheet="1" windowHeight="7755" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
@@ -18,14 +18,15 @@
     <sheet name="CreateUser" r:id="rId4" sheetId="2"/>
     <sheet name="GroupDetails" r:id="rId5" sheetId="3"/>
     <sheet name="CreateEmployee" r:id="rId6" sheetId="4"/>
-    <sheet name="DocumentRoutes" r:id="rId7" sheetId="5"/>
+    <sheet name="PeriodicReviewer" r:id="rId7" sheetId="21"/>
+    <sheet name="DocumentRoutes" r:id="rId8" sheetId="5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="122">
   <si>
     <t>Admin</t>
   </si>
@@ -364,6 +365,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Check in User</t>
+  </si>
+  <si>
+    <t>ANT-FORM</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>ANT-SOP</t>
+  </si>
+  <si>
+    <t>Actions required by doc Owner</t>
+  </si>
+  <si>
+    <t>DocTitleSummary</t>
+  </si>
+  <si>
+    <t>periodicReviewsDays</t>
+  </si>
+  <si>
+    <t>approveComment</t>
+  </si>
+  <si>
+    <t>Changes Required</t>
   </si>
 </sst>
 </file>
@@ -818,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1019,6 +1047,17 @@
         <v>107</v>
       </c>
     </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -1030,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1508,10 +1547,58 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>